<commit_message>
[UPDATE] finishing role admin
</commit_message>
<xml_diff>
--- a/public/Template Upload User.xlsx
+++ b/public/Template Upload User.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mirza\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\simta\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96236AB-05DC-4E53-8614-72BCBB849542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE18AF6B-E1B6-4199-B71A-FFAD2D1B3A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,9 +48,6 @@
     <t>gungun@gmail.com</t>
   </si>
   <si>
-    <t>gungun123</t>
-  </si>
-  <si>
     <t>Riski Putri</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>mahasiswa</t>
+  </si>
+  <si>
+    <t>gunawan123</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +445,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -456,16 +456,16 @@
         <v>2131741124</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -473,16 +473,16 @@
         <v>2131741125</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>